<commit_message>
updated sql, added staffverification modal via button,completed file upload
</commit_message>
<xml_diff>
--- a/uploaded_files/Master.xlsx
+++ b/uploaded_files/Master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF5B919-7CBE-422C-9214-D2BC6C9768F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2163B963-3CD7-4847-9C6C-FF186C1B444A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18480" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Supervisor</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Sourav Saha Bhowmick</t>
+  </si>
+  <si>
+    <t>Sun Aixin</t>
+  </si>
+  <si>
+    <t>Ta Nguyen Binh Duong</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -128,6 +134,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,9 +444,7 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -445,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -453,28 +460,24 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>2</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -495,11 +498,22 @@
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="4">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>